<commit_message>
feat(LTS): Simple Model V2 (full)
The remaining code for the Simple Model V2 (i.e., the dynamics, the path constraints and the cost, as well as some other minor changes) is included.

Note that the solver DOES NOT CONVERGE with this model.
</commit_message>
<xml_diff>
--- a/LTS_inputData.xlsx
+++ b/LTS_inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kreisler\Documents\MATLAB\ICLOCS-master\usr\LTS Problem\LTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA825A99-F27F-4B97-9D93-02677EEFEDB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BECD80F-DD59-4F6A-8188-8A1C9CC36BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E3DC8AB-017F-425C-8100-FA3250F23AF7}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="133">
   <si>
     <t>m</t>
   </si>
@@ -159,30 +159,6 @@
     <t>Control</t>
   </si>
   <si>
-    <t>YAS left paddle position</t>
-  </si>
-  <si>
-    <t>\theta_{yl}</t>
-  </si>
-  <si>
-    <t>YAS right paddle position</t>
-  </si>
-  <si>
-    <t>\theta_{yr}</t>
-  </si>
-  <si>
-    <t>Brake pedal position</t>
-  </si>
-  <si>
-    <t>\theta_b</t>
-  </si>
-  <si>
-    <t>Throttle pedal position</t>
-  </si>
-  <si>
-    <t>\theta_t</t>
-  </si>
-  <si>
     <t>Steering wheel angle</t>
   </si>
   <si>
@@ -315,9 +291,6 @@
     <t>Int. tol. Abs.</t>
   </si>
   <si>
-    <t>Angle track orientation &gt; vehicle heading</t>
-  </si>
-  <si>
     <t>bConst. Tol</t>
   </si>
   <si>
@@ -426,24 +399,12 @@
     <t>lateral shape factor</t>
   </si>
   <si>
-    <t>mu_x1</t>
-  </si>
-  <si>
-    <t>mu_x2</t>
-  </si>
-  <si>
     <t>kappa_1</t>
   </si>
   <si>
     <t>kappa_2</t>
   </si>
   <si>
-    <t>mu_y1</t>
-  </si>
-  <si>
-    <t>mu_y2</t>
-  </si>
-  <si>
     <t>alpha_1</t>
   </si>
   <si>
@@ -463,6 +424,54 @@
   </si>
   <si>
     <t>weight</t>
+  </si>
+  <si>
+    <t>\kappa_fr</t>
+  </si>
+  <si>
+    <t>\kappa_fl</t>
+  </si>
+  <si>
+    <t>\kappa_rr</t>
+  </si>
+  <si>
+    <t>\kappa_rl</t>
+  </si>
+  <si>
+    <t>Slip ratio - fr tyre</t>
+  </si>
+  <si>
+    <t>Slip ratio - fl tyre</t>
+  </si>
+  <si>
+    <t>Slip ratio - rr tyre</t>
+  </si>
+  <si>
+    <t>Slip ratio - rl tyre</t>
+  </si>
+  <si>
+    <t>º</t>
+  </si>
+  <si>
+    <t>mux_1</t>
+  </si>
+  <si>
+    <t>mux_2</t>
+  </si>
+  <si>
+    <t>muy_1</t>
+  </si>
+  <si>
+    <t>muy_2</t>
+  </si>
+  <si>
+    <t>kbb</t>
+  </si>
+  <si>
+    <t>front brake bias</t>
+  </si>
+  <si>
+    <t>Angle track orientation to vehicle heading</t>
   </si>
 </sst>
 </file>
@@ -473,7 +482,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.###"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,12 +497,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -915,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCC6EC8-B294-4B15-BEFB-0F1B38D6C8F3}">
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,70 +935,70 @@
   <sheetData>
     <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -1003,41 +1006,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J2" s="9">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="K2" s="9">
-        <f>J2</f>
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="N2" s="12">
         <v>0</v>
@@ -1052,10 +1054,10 @@
         <v>20</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="T2" s="9">
         <v>0</v>
@@ -1064,7 +1066,7 @@
         <v>100</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="W2" s="9"/>
       <c r="X2" s="9"/>
@@ -1077,16 +1079,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F3" s="9">
         <f>-G3</f>
@@ -1097,42 +1099,41 @@
         <v>2.1349999999999998</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J3" s="9">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="K3" s="9">
-        <f t="shared" ref="K3:K7" si="0">J3</f>
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="L3" s="9">
         <f>G3/50</f>
         <v>4.2699999999999995E-2</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>20</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="10" t="s">
         <v>20</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="T3" s="9">
         <v>0</v>
@@ -1143,7 +1144,7 @@
       </c>
       <c r="V3" s="9">
         <f>J3</f>
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
@@ -1156,74 +1157,72 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F4" s="10">
         <f>-G4</f>
-        <v>-1.5707963267948966</v>
+        <v>-1.2566370614359172</v>
       </c>
       <c r="G4" s="9">
-        <f>PI()/2</f>
-        <v>1.5707963267948966</v>
+        <f>PI()/2*0.8</f>
+        <v>1.2566370614359172</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J4" s="9">
-        <f>RADIANS(0.5)</f>
-        <v>8.7266462599716477E-3</v>
+        <v>1</v>
       </c>
       <c r="K4" s="9">
-        <f t="shared" si="0"/>
-        <v>8.7266462599716477E-3</v>
+        <v>1</v>
       </c>
       <c r="L4" s="9">
         <f>G4/50</f>
-        <v>3.1415926535897934E-2</v>
+        <v>2.5132741228718346E-2</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>20</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="10" t="s">
         <v>20</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="T4" s="9">
         <v>0</v>
       </c>
       <c r="U4" s="9">
-        <f t="shared" ref="U4:U12" si="1">T4</f>
+        <f t="shared" ref="U4:U12" si="0">T4</f>
         <v>0</v>
       </c>
       <c r="V4" s="9">
-        <f t="shared" ref="V4:V7" si="2">J4</f>
-        <v>8.7266462599716477E-3</v>
+        <f t="shared" ref="V4:V7" si="1">J4</f>
+        <v>1</v>
       </c>
       <c r="W4" s="9"/>
       <c r="X4" s="9"/>
@@ -1236,71 +1235,69 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F5" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J5" s="9">
-        <f>T5/100</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="K5" s="9">
+        <v>1</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="9">
+        <v>20</v>
+      </c>
+      <c r="U5" s="9">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="T5" s="9">
-        <v>20</v>
-      </c>
-      <c r="U5" s="9">
+        <v>20</v>
+      </c>
+      <c r="V5" s="9">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="V5" s="9">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
@@ -1313,70 +1310,69 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J6" s="9">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="K6" s="9">
+        <v>1</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="9">
+        <v>0</v>
+      </c>
+      <c r="U6" s="9">
         <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="T6" s="9">
-        <v>0</v>
-      </c>
-      <c r="U6" s="9">
+        <v>0</v>
+      </c>
+      <c r="V6" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V6" s="9">
-        <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
@@ -1389,70 +1385,69 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J7" s="9">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="K7" s="9">
+        <v>1</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="9">
+        <v>0</v>
+      </c>
+      <c r="U7" s="9">
         <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="S7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="T7" s="9">
-        <v>0</v>
-      </c>
-      <c r="U7" s="9">
+        <v>0</v>
+      </c>
+      <c r="V7" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="9">
-        <f t="shared" si="2"/>
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="W7" s="9"/>
       <c r="X7" s="9"/>
@@ -1465,10 +1460,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>20</v>
@@ -1485,10 +1480,10 @@
         <v>3.1415926535897931</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -1504,25 +1499,25 @@
         <v>20</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="R8" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="T8" s="9">
         <v>0</v>
       </c>
       <c r="U8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V8" s="9">
@@ -1540,10 +1535,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>20</v>
@@ -1551,56 +1546,53 @@
       <c r="E9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>1</v>
+      <c r="F9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
-      <c r="L9" s="9">
-        <f t="shared" ref="L9:L12" si="3">G9/50</f>
-        <v>0.02</v>
-      </c>
-      <c r="M9" s="9">
-        <f t="shared" ref="M9:M12" si="4">G9/5</f>
-        <v>0.2</v>
+      <c r="L9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="N9" s="10" t="s">
         <v>20</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q9" s="10" t="s">
         <v>20</v>
       </c>
       <c r="R9" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="T9" s="9">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="U9" s="9">
-        <f t="shared" si="1"/>
-        <v>0.7</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="V9" s="9">
-        <f t="shared" ref="V9:V12" si="5">L9</f>
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
@@ -1613,10 +1605,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>20</v>
@@ -1624,56 +1616,53 @@
       <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="9">
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <v>1</v>
+      <c r="F10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="9">
-        <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="M10" s="9">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
+      <c r="L10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="R10" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="T10" s="9">
         <v>0</v>
       </c>
       <c r="U10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="V10" s="9">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
@@ -1686,10 +1675,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>20</v>
@@ -1697,56 +1686,54 @@
       <c r="E11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="9">
-        <v>0</v>
-      </c>
-      <c r="G11" s="9">
-        <v>1</v>
+      <c r="F11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="9">
-        <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="M11" s="9">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
+      <c r="L11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="N11" s="10" t="s">
         <v>20</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q11" s="10" t="s">
         <v>20</v>
       </c>
       <c r="R11" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="T11" s="9">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="U11" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="V11" s="9">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
+        <f>T11/10</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
@@ -1759,10 +1746,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>20</v>
@@ -1770,62 +1757,116 @@
       <c r="E12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>1</v>
+      <c r="F12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
-      <c r="L12" s="9">
-        <f t="shared" si="3"/>
-        <v>0.02</v>
-      </c>
-      <c r="M12" s="9">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
+      <c r="L12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="N12" s="10" t="s">
         <v>20</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q12" s="10" t="s">
         <v>20</v>
       </c>
       <c r="R12" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="T12" s="9">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="U12" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="V12" s="9">
-        <f t="shared" si="5"/>
-        <v>0.02</v>
+        <f>T12/10</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="W12" s="9"/>
       <c r="X12" s="9"/>
       <c r="Y12" s="9"/>
       <c r="Z12" s="9"/>
       <c r="AA12" s="9"/>
+    </row>
+    <row r="21" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K21" s="9">
+        <f>J21</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="K22" s="9">
+        <f t="shared" ref="K22:K26" si="2">J22</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="9">
+        <f>RADIANS(0.5)</f>
+        <v>8.7266462599716477E-3</v>
+      </c>
+      <c r="K23" s="9">
+        <f t="shared" si="2"/>
+        <v>8.7266462599716477E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="9">
+        <f>T24/100</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="K25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="26" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="K26" s="9">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
@@ -1851,15 +1892,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B2">
         <v>2.5</v>
@@ -1876,10 +1917,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B734AD-4E25-43B0-B54F-08325C747299}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,30 +1931,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C2" s="3">
         <v>9.81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,22 +1973,22 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C4">
         <f>C2*C3</f>
         <v>6474.6</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -1956,7 +1997,7 @@
         <v>450</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,7 +2059,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -2032,7 +2073,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -2046,7 +2087,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -2074,7 +2115,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -2083,12 +2124,12 @@
         <v>10.47</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -2103,7 +2144,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
@@ -2118,7 +2159,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -2132,7 +2173,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -2146,7 +2187,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -2161,30 +2202,44 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C20">
         <v>1000</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C21">
         <v>20000</v>
       </c>
       <c r="D21" t="s">
-        <v>97</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22">
+        <v>0.45</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2203,8 +2258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8F6FFE-7F11-44DA-B81A-BB53F53A623D}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,108 +2270,108 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C2">
         <v>2000</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C3">
         <v>6000</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C4">
         <v>1.75</v>
       </c>
-      <c r="D4" t="s">
-        <v>0</v>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>1.4</v>
       </c>
-      <c r="D5" t="s">
-        <v>0</v>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>0.11</v>
       </c>
-      <c r="D6" t="s">
-        <v>0</v>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C7">
         <v>0.1</v>
       </c>
-      <c r="D7" t="s">
-        <v>0</v>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>1.8</v>
@@ -2327,72 +2382,72 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C9">
         <v>1.45</v>
       </c>
-      <c r="D9" t="s">
-        <v>0</v>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
-        <v>0</v>
+      <c r="D10" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>0</v>
+      <c r="D11" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C12">
         <v>1.9</v>
       </c>
-      <c r="D12" t="s">
-        <v>94</v>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C13">
         <v>1.9</v>
       </c>
-      <c r="D13" t="s">
-        <v>24</v>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(LTS): Simple Model V2 -better convergence-
5 actions listed in the user guide are taken to improve convergence, including deactivating some constraints or refining the initial guesses.

A satisfactory (feasible) solution is still not found.
</commit_message>
<xml_diff>
--- a/LTS_inputData.xlsx
+++ b/LTS_inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kreisler\Documents\MATLAB\ICLOCS-master\usr\LTS Problem\LTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BECD80F-DD59-4F6A-8188-8A1C9CC36BF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2684FE8D-CFC3-46B8-8E23-99BCC1D7C1F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E3DC8AB-017F-425C-8100-FA3250F23AF7}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="132">
   <si>
     <t>m</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>TC bound U</t>
   </si>
   <si>
@@ -369,24 +366,6 @@
     <t>reference load 2</t>
   </si>
   <si>
-    <t>peak longitudinal friction coe_x000E_cient at load 1</t>
-  </si>
-  <si>
-    <t>peak longitudinal friction coe_x000E_cient at load 2</t>
-  </si>
-  <si>
-    <t>slip coe_x000E_cient for the friction peak at load 1</t>
-  </si>
-  <si>
-    <t>slip coe_x000E_cient for the friction peak at load 2</t>
-  </si>
-  <si>
-    <t>peak lateral friction coe_x000E_cient at load 1</t>
-  </si>
-  <si>
-    <t>peak lateral friction coe_x000E_cient at load 2</t>
-  </si>
-  <si>
     <t>slip angle for the friction peak at load 1</t>
   </si>
   <si>
@@ -472,6 +451,24 @@
   </si>
   <si>
     <t>Angle track orientation to vehicle heading</t>
+  </si>
+  <si>
+    <t>slip coefficient for the friction peak at load 1</t>
+  </si>
+  <si>
+    <t>slip coefficient for the friction peak at load 2</t>
+  </si>
+  <si>
+    <t>peak lateral friction coefficient at load 1</t>
+  </si>
+  <si>
+    <t>peak lateral friction coefficient at load 2</t>
+  </si>
+  <si>
+    <t>peak longitudinal friction coefficient at load 2</t>
+  </si>
+  <si>
+    <t>peak longitudinal friction coefficient at load 1</t>
   </si>
 </sst>
 </file>
@@ -921,7 +918,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,70 +932,70 @@
   <sheetData>
     <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -1006,7 +1003,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>46</v>
@@ -1017,11 +1014,11 @@
       <c r="E2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>43</v>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9">
+        <v>200</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>44</v>
@@ -1091,12 +1088,10 @@
         <v>30</v>
       </c>
       <c r="F3" s="9">
-        <f>-G3</f>
-        <v>-2.1349999999999998</v>
+        <v>0</v>
       </c>
       <c r="G3" s="9">
-        <f>trackInput!B2-MAX(carInput!C11,carInput!C12)/2</f>
-        <v>2.1349999999999998</v>
+        <v>0</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>44</v>
@@ -1112,7 +1107,7 @@
       </c>
       <c r="L3" s="9">
         <f>G3/50</f>
-        <v>4.2699999999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>43</v>
@@ -1160,7 +1155,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>39</v>
@@ -1176,11 +1171,11 @@
         <f>PI()/2*0.8</f>
         <v>1.2566370614359172</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>43</v>
+      <c r="H4" s="10">
+        <v>-5</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5</v>
       </c>
       <c r="J4" s="9">
         <v>1</v>
@@ -1192,8 +1187,8 @@
         <f>G4/50</f>
         <v>2.5132741228718346E-2</v>
       </c>
-      <c r="M4" s="9" t="s">
-        <v>43</v>
+      <c r="M4" s="9">
+        <v>0.1</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>20</v>
@@ -1247,16 +1242,16 @@
         <v>30</v>
       </c>
       <c r="F5" s="9">
-        <v>2</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>43</v>
+        <v>5</v>
+      </c>
+      <c r="G5" s="10">
+        <v>100</v>
+      </c>
+      <c r="H5" s="10">
+        <v>-20</v>
+      </c>
+      <c r="I5" s="9">
+        <v>20</v>
       </c>
       <c r="J5" s="9">
         <v>1</v>
@@ -1264,11 +1259,11 @@
       <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>43</v>
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5" s="9">
+        <v>1</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>20</v>
@@ -1321,17 +1316,17 @@
       <c r="E6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>43</v>
+      <c r="F6" s="10">
+        <v>-50</v>
+      </c>
+      <c r="G6" s="9">
+        <v>50</v>
+      </c>
+      <c r="H6" s="10">
+        <v>-50</v>
+      </c>
+      <c r="I6" s="9">
+        <v>50</v>
       </c>
       <c r="J6" s="9">
         <v>1</v>
@@ -1339,11 +1334,11 @@
       <c r="K6" s="9">
         <v>1</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>43</v>
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9">
+        <v>1</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>20</v>
@@ -1396,17 +1391,17 @@
       <c r="E7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>43</v>
+      <c r="F7" s="10">
+        <v>-50</v>
+      </c>
+      <c r="G7" s="9">
+        <v>50</v>
+      </c>
+      <c r="H7" s="10">
+        <v>-10</v>
+      </c>
+      <c r="I7" s="9">
+        <v>10</v>
       </c>
       <c r="J7" s="9">
         <v>1</v>
@@ -1414,11 +1409,11 @@
       <c r="K7" s="9">
         <v>1</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>43</v>
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
+      <c r="M7" s="9">
+        <v>1</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>20</v>
@@ -1479,11 +1474,11 @@
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>43</v>
+      <c r="H8" s="10">
+        <v>-3</v>
+      </c>
+      <c r="I8" s="9">
+        <v>3</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -1535,10 +1530,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>20</v>
@@ -1546,25 +1541,26 @@
       <c r="E9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>43</v>
+      <c r="F9" s="10">
+        <v>-2</v>
+      </c>
+      <c r="G9" s="9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="10">
+        <f>-I9</f>
+        <v>-2</v>
+      </c>
+      <c r="I9" s="9">
+        <v>2</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
-      <c r="L9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>43</v>
+      <c r="L9" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="9">
+        <v>1</v>
       </c>
       <c r="N9" s="10" t="s">
         <v>20</v>
@@ -1605,10 +1601,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>20</v>
@@ -1616,25 +1612,26 @@
       <c r="E10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>43</v>
+      <c r="F10" s="10">
+        <v>-2</v>
+      </c>
+      <c r="G10" s="9">
+        <v>2</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" ref="H10:H12" si="2">-I10</f>
+        <v>-2</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>43</v>
+      <c r="L10" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="M10" s="9">
+        <v>1</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>20</v>
@@ -1675,10 +1672,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>20</v>
@@ -1686,25 +1683,26 @@
       <c r="E11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>43</v>
+      <c r="F11" s="10">
+        <v>-2</v>
+      </c>
+      <c r="G11" s="9">
+        <v>2</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="I11" s="9">
+        <v>2</v>
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
-      <c r="L11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>43</v>
+      <c r="L11" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="M11" s="9">
+        <v>1</v>
       </c>
       <c r="N11" s="10" t="s">
         <v>20</v>
@@ -1746,10 +1744,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>20</v>
@@ -1757,25 +1755,26 @@
       <c r="E12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>43</v>
+      <c r="F12" s="10">
+        <v>-2</v>
+      </c>
+      <c r="G12" s="9">
+        <v>2</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="I12" s="9">
+        <v>2</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
-      <c r="L12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>43</v>
+      <c r="L12" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="9">
+        <v>1</v>
       </c>
       <c r="N12" s="10" t="s">
         <v>20</v>
@@ -1826,7 +1825,7 @@
         <v>0.01</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" ref="K22:K26" si="2">J22</f>
+        <f t="shared" ref="K22:K26" si="3">J22</f>
         <v>0.01</v>
       </c>
     </row>
@@ -1836,7 +1835,7 @@
         <v>8.7266462599716477E-3</v>
       </c>
       <c r="K23" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.7266462599716477E-3</v>
       </c>
     </row>
@@ -1846,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -1855,7 +1854,7 @@
         <v>0.05</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
     </row>
@@ -1864,7 +1863,7 @@
         <v>0.05</v>
       </c>
       <c r="K26" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
     </row>
@@ -1885,25 +1884,25 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2">
-        <v>2.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1919,7 +1918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B734AD-4E25-43B0-B54F-08325C747299}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1931,30 +1930,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C2" s="3">
         <v>9.81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1973,22 +1972,22 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C4">
         <f>C2*C3</f>
         <v>6474.6</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -1997,7 +1996,7 @@
         <v>450</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2059,7 +2058,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -2073,7 +2072,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -2087,7 +2086,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -2115,7 +2114,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -2124,12 +2123,12 @@
         <v>10.47</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -2144,7 +2143,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
@@ -2159,7 +2158,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -2173,7 +2172,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -2187,7 +2186,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -2202,38 +2201,38 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20">
         <v>1000</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21">
         <v>20000</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C22">
         <v>0.45</v>
@@ -2259,7 +2258,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,52 +2269,52 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>2000</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3">
         <v>6000</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="C4">
         <v>1.75</v>
@@ -2326,10 +2325,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="C5">
         <v>1.4</v>
@@ -2340,10 +2339,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="C6">
         <v>0.11</v>
@@ -2354,10 +2353,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="C7">
         <v>0.1</v>
@@ -2368,10 +2367,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
         <v>128</v>
-      </c>
-      <c r="B8" t="s">
-        <v>102</v>
       </c>
       <c r="C8">
         <v>1.8</v>
@@ -2382,10 +2381,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
         <v>129</v>
-      </c>
-      <c r="B9" t="s">
-        <v>103</v>
       </c>
       <c r="C9">
         <v>1.45</v>
@@ -2396,38 +2395,38 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C12">
         <v>1.9</v>
@@ -2438,10 +2437,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C13">
         <v>1.9</v>

</xml_diff>

<commit_message>
fix(LTS_dynamics): Error in units
Error in \alpha units (rad instead of deg to compare with \alpha_max) fixed.
</commit_message>
<xml_diff>
--- a/LTS_inputData.xlsx
+++ b/LTS_inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kreisler\Documents\MATLAB\ICLOCS-master\usr\LTS Problem\LTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2684FE8D-CFC3-46B8-8E23-99BCC1D7C1F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7D7254-EFE5-4D34-BED8-2CD4AC613348}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E3DC8AB-017F-425C-8100-FA3250F23AF7}"/>
+    <workbookView xWindow="-21396" yWindow="1056" windowWidth="19680" windowHeight="10584" xr2:uid="{8E3DC8AB-017F-425C-8100-FA3250F23AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="numericsInput" sheetId="2" r:id="rId1"/>
@@ -549,7 +549,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -918,7 +962,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,7 +1913,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2243,7 +2287,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2451,7 +2495,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>